<commit_message>
Conveqs hidden release. New output format: grammar sketch Comments for sentence pairs
</commit_message>
<xml_diff>
--- a/templates/sentence_pairs_template.xlsx
+++ b/templates/sentence_pairs_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastienchristian/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastienchristian/Desktop/d/01-These/Engine/v1/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B2A1451-0463-864C-BA6D-AABCBF0F7110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA571C7B-FEF1-C940-8145-EF37FD78E80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1220" windowWidth="10960" windowHeight="14600" xr2:uid="{22C1F765-0B47-A94E-8B49-5FB55A6316FC}"/>
+    <workbookView xWindow="3620" yWindow="1220" windowWidth="15680" windowHeight="14600" xr2:uid="{22C1F765-0B47-A94E-8B49-5FB55A6316FC}"/>
   </bookViews>
   <sheets>
     <sheet name="sentence_pairs_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>source</t>
   </si>
@@ -50,13 +50,28 @@
   </si>
   <si>
     <t>sentence 4 in the target language</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>comments about sentence 1</t>
+  </si>
+  <si>
+    <t>comments about sentence 2</t>
+  </si>
+  <si>
+    <t>comments about sentence 3</t>
+  </si>
+  <si>
+    <t>comments about sentence 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,6 +202,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -890,59 +911,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014CDB78-685F-1B45-A768-2FFC7E2DFFB5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.6640625" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>